<commit_message>
fixed up the excel and csv files so they properly export to postgres
</commit_message>
<xml_diff>
--- a/Databases/MobiedockDataFiles/Excel Tables:Other Docs/BayAvaliable.xlsx
+++ b/Databases/MobiedockDataFiles/Excel Tables:Other Docs/BayAvaliable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nico/Desktop/solar-scooter-project/Databases/MobiedockDataFiles/Excel Tables:Other Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bendavis/Documents/solar-scooter-project/Databases/MobiedockDataFiles/Excel Tables:Other Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334CC0D3-CAFA-8D47-9CE2-964F65BDDA3E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA90295-0CAF-4746-8DBA-C6D2F9719F03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="460" windowWidth="12100" windowHeight="15540" xr2:uid="{3DBFEC15-2A34-1642-85F3-3CC2FE786350}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>1B1</t>
   </si>
@@ -117,10 +117,19 @@
     <t>5B6</t>
   </si>
   <si>
-    <t>bay_id</t>
-  </si>
-  <si>
-    <t>availability</t>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
   </si>
 </sst>
 </file>
@@ -472,260 +481,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE685F5-65E1-014C-BFB4-5E2878919519}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="b">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C1048576" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>